<commit_message>
Re-write the R script using lapply and mapply.
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Xixi/Work/Papers/190606 Katie AUM miRNA/Uranium-miRNA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A6C4CF-45D0-9E4E-BE4C-3828D55BB0A8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D53003-EE16-8B45-9349-34EDECBC88DB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2360" yWindow="800" windowWidth="28040" windowHeight="17440" xr2:uid="{DA1D7875-D6FB-C142-BE92-EB44806D0A66}"/>
   </bookViews>
@@ -80,7 +80,7 @@
     <t>miRNA</t>
   </si>
   <si>
-    <t>Regulation</t>
+    <t>regulation</t>
   </si>
 </sst>
 </file>
@@ -439,7 +439,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>